<commit_message>
finished app to label reverb entities
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -72,9 +72,6 @@
     <t>/m/0dwzk4 Chadian-Libyan conflict 97</t>
   </si>
   <si>
-    <t>Williams</t>
-  </si>
-  <si>
     <t>/m/086x3 WilliamsF1 2930</t>
   </si>
   <si>
@@ -1702,6 +1699,9 @@
   </si>
   <si>
     <t>bad reverb entry</t>
+  </si>
+  <si>
+    <t>Willaims</t>
   </si>
 </sst>
 </file>
@@ -2087,8 +2087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B803"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B797" sqref="B797"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="B181" sqref="B181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2189,88 +2189,88 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>561</v>
       </c>
       <c r="B19" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2295,313 +2295,313 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B70" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B75" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B81" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -2611,961 +2611,961 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B113" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B115" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B123" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B130" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B134" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B142" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B147" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B169" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B173" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B187" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B192" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B195" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B201" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B204" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B210" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B211" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B214" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B219" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B220" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B223" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B226" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B229" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B230" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B231" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B232" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B233" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B234" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B235" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B237" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B238" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B239" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B240" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B241" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B242" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B243" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B244" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B245" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B246" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B247" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B248" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B250" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B251" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B252" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B253" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B254" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B256" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B257" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B258" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B259" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B260" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B261" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B262" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B263" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B264" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B266" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B267" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B268" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B269" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B270" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B272" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B273" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B274" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B275" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B276" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B278" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B279" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B280" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B281" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B282" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B284" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
@@ -3575,47 +3575,47 @@
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B286" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B287" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B288" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B290" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B291" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B292" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B293" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B294" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
@@ -3650,157 +3650,157 @@
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B302" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B303" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B304" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B305" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B306" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B308" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B309" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B310" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B311" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B312" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B314" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B315" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B317" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B318" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B319" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B321" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B322" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B323" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B324" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B325" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B327" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B328" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B329" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B330" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B331" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
@@ -3830,127 +3830,127 @@
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B337" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B339" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B340" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B341" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B342" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B343" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A344" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B345" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B346" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B347" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B348" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B349" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B351" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B352" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B353" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B354" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A355" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B356" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B357" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B358" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B359" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B360" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A361" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
@@ -3960,67 +3960,67 @@
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B363" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B364" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B365" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B366" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A367" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B368" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B369" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B370" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B371" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B372" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B374" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A375" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
@@ -4045,40 +4045,40 @@
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B380" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B381" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B382" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B383" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B384" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B385" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B386" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
@@ -4113,37 +4113,37 @@
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A393" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B394" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B395" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B396" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B397" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B398" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A399" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
@@ -4153,322 +4153,322 @@
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B402" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A403" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B404" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B405" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B406" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B407" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B408" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A409" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B410" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B411" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B412" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B413" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B414" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A415" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B416" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B417" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B418" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B419" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B420" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A421" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B422" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B423" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B424" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B425" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B426" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A427" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B428" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B429" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B430" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B431" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B432" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A433" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B434" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B435" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B436" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B437" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B438" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A439" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B440" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B441" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A442" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B443" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B444" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B445" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B446" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B447" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A448" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B449" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B450" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B451" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A452" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B453" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B454" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B455" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B456" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B457" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A458" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B459" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B460" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B461" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B462" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B463" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A464" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.25">
@@ -4478,455 +4478,455 @@
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B466" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B467" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B468" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B469" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A470" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B471" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B472" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B473" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B474" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="475" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B475" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A476" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B476" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B477" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B478" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B479" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B480" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B481" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A482" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B483" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B484" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B485" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B486" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B487" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A488" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B489" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B490" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B491" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B492" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B493" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A494" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B495" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B496" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B497" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B498" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B499" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A500" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B501" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B502" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B503" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B504" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B505" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A506" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B507" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A508" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B509" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B510" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B511" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B512" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B513" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A514" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="515" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B515" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="516" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B516" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="517" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B517" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="518" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B518" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="519" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B519" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="520" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A520" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="521" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B521" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B522" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B523" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B524" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="525" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B525" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="526" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A526" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="527" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B527" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B528" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B529" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="530" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B530" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="531" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B531" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="532" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A532" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="533" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B533" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="534" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B534" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="535" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B535" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="536" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B536" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="537" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B537" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="538" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A538" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="539" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B539" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="540" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B540" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="541" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B541" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="542" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B542" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="543" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B543" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="544" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A544" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="545" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B545" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B546" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="547" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B547" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="548" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B548" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="549" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B549" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="550" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A550" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="551" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B551" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="552" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B552" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="553" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B553" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="554" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B554" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="555" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B555" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="556" spans="1:2" x14ac:dyDescent="0.25">
@@ -4961,216 +4961,216 @@
     </row>
     <row r="562" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A562" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="563" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B563" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="564" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B564" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="565" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B565" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="566" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B566" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="567" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B567" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="568" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A568" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B568" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="569" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B569" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="570" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A570" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B570" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="571" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B571" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="572" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B572" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="573" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A573" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="574" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B574" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="575" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B575" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="576" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B576" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="577" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B577" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="578" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B578" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="579" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A579" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="580" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B580" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="581" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B581" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="582" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B582" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="583" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B583" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="584" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B584" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="585" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A585" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B585" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="586" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B586" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="587" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B587" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="588" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B588" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="589" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B589" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="590" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B590" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="591" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A591" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="592" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B592" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="593" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B593" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="594" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B594" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="595" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B595" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="596" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B596" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="597" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A597" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B598" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="599" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B599" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="600" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B600" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="601" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B601" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="602" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B602" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="603" spans="1:2" x14ac:dyDescent="0.25">
@@ -5205,437 +5205,437 @@
     </row>
     <row r="609" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A609" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B609" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="610" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B610" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="611" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B611" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="612" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B612" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="613" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B613" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="614" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B614" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="615" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A615" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="616" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B616" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="617" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B617" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="618" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B618" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="619" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B619" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="620" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B620" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A621" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B621" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B622" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A623" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B624" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="625" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B625" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="626" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B626" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="627" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B627" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="628" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B628" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="629" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A629" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="630" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B630" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="631" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B631" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="632" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B632" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="633" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B633" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="634" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B634" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="635" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A635" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="636" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B636" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="637" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B637" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="638" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B638" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="639" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B639" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="640" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B640" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="641" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A641" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B642" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B643" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B644" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="645" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B645" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="646" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B646" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="647" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A647" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B648" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B649" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B650" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B651" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B652" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A653" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B653" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B654" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B655" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B656" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="657" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B657" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="658" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B658" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="659" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A659" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="660" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B660" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="661" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B661" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="662" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B662" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="663" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B663" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="664" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A664" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="665" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B665" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="666" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B666" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="667" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B667" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="668" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B668" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="669" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B669" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="670" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A670" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B670" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="671" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B671" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="672" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B672" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="673" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B673" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="674" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B674" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="675" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B675" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A676" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B677" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B678" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B679" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="680" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B680" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="681" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B681" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A682" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B682" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="683" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B683" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B684" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="685" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A685" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="686" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B686" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="687" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B687" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="688" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B688" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="689" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B689" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="690" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B690" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="691" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A691" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B692" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="693" spans="1:2" x14ac:dyDescent="0.25">
@@ -5645,92 +5645,92 @@
     </row>
     <row r="694" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B694" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="695" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B695" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="696" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B696" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="697" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A697" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="698" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B698" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="699" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B699" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="700" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B700" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="701" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B701" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B702" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A703" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B704" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="705" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B705" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="706" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B706" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="707" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B707" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="708" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B708" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="709" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A709" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="710" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B710" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B711" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.25">
@@ -5740,490 +5740,490 @@
     </row>
     <row r="713" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B713" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B714" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A715" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B715" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="716" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B716" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="717" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B717" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B718" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A719" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B720" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="721" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B721" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="722" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A722" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B722" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="723" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B723" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="724" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B724" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B725" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B726" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B727" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A728" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B729" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B730" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="731" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B731" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="732" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B732" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="733" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B733" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="734" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A734" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="735" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B735" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B736" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A737" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B738" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B739" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B740" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B741" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A742" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B742" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="743" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B743" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B744" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B745" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B746" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B747" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A748" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B748" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="749" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B749" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="750" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B750" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="751" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B751" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="752" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B752" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="753" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B753" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="754" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A754" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="755" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B755" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="756" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B756" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="757" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B757" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="758" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B758" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="759" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B759" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="760" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A760" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B760" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="761" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B761" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="762" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B762" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="763" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B763" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="764" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B764" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="765" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B765" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="766" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A766" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B766" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="767" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B767" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="768" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B768" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="769" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B769" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="770" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B770" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="771" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B771" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="772" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A772" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="773" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B773" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="774" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B774" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="775" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B775" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="776" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A776" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B776" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="777" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B777" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="778" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B778" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="779" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A779" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B779" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="780" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B780" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="781" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B781" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="782" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B782" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="783" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B783" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="784" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B784" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="785" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A785" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B785" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="786" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B786" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="787" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B787" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="788" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B788" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="789" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B789" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="790" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B790" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="791" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A791" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="792" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B792" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="793" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B793" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="794" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B794" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="795" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B795" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="796" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B796" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="797" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A797" s="2" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="797" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A797" s="1" t="s">
-        <v>536</v>
-      </c>
       <c r="B797" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="798" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B798" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="799" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B799" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="800" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B800" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="801" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B801" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="802" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B802" s="2" t="s">
         <v>539</v>
-      </c>
-    </row>
-    <row r="802" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B802" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="803" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A803" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B803" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
   </sheetData>

</xml_diff>